<commit_message>
Share Skill added,Edit and Delete in Manage Listing.
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Testing\Tester\Competitive-tasks\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428059-39C0-4B90-8BCF-7E49202B9138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00D85E3-7871-4CEC-8E00-644570F1514F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SignUp" sheetId="3" r:id="rId1"/>
-    <sheet name="SignIn" sheetId="1" r:id="rId2"/>
-    <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="ShareSkill" sheetId="7" r:id="rId1"/>
+    <sheet name="EditShareSkill" sheetId="6" r:id="rId2"/>
+    <sheet name="ManageListings" sheetId="4" r:id="rId3"/>
+    <sheet name="SignUp" sheetId="3" r:id="rId4"/>
+    <sheet name="SignIn" sheetId="1" r:id="rId5"/>
+    <sheet name="Profile" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Url</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>http://www.skillswap.pro/Home</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -93,37 +93,140 @@
     <t>ConfirmPswd</t>
   </si>
   <si>
-    <t>Venugan</t>
-  </si>
-  <si>
-    <t>Vidhya</t>
-  </si>
-  <si>
-    <t>vidhyav9@gmail.com</t>
-  </si>
-  <si>
-    <t>Ithika2015</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>Melbourne</t>
-  </si>
-  <si>
-    <t>Amrita School Of Engineering</t>
-  </si>
-  <si>
-    <t>B.Tech</t>
-  </si>
-  <si>
-    <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>Jawaharlal Nehru Technological University</t>
+  </si>
+  <si>
+    <t>M.Tech</t>
+  </si>
+  <si>
+    <t>1 and half year experience in Manual testing</t>
+  </si>
+  <si>
+    <t>http://localhost:5000</t>
+  </si>
+  <si>
+    <t>priyanka.mekha@gmail.com</t>
+  </si>
+  <si>
+    <t>Bollepalli88</t>
+  </si>
+  <si>
+    <t>Priyanka</t>
+  </si>
+  <si>
+    <t>Meka</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>19:00:00 PM</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>Would like to provide Python training for beginners</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Would like to provide selenium training for beginners</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Thurs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,10 +273,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -512,54 +620,340 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4B586F-B3AC-47CB-A5C1-6F1CC71A7338}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="20.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="5">
+        <v>44663</v>
+      </c>
+      <c r="I2" s="6">
+        <v>44693</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E8C687-A4B2-47D9-9132-648FB3D1D713}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="42.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44663</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44724</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969C4D49-DA18-4326-B45D-53AACFF13E8C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -570,22 +964,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,110 +990,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="Test@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId2" display="Test@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="1" max="3" width="20.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="10" max="10" width="52.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>